<commit_message>
Begin reorganize workers. Split to some massive
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -122,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6471">
+  <cellXfs count="6223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -5236,254 +5236,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
@@ -6854,13 +6606,13 @@
       <c r="O4" s="5155" t="n">
         <v>8.0</v>
       </c>
-      <c r="P4" s="5159" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="P4" s="5161"/>
       <c r="Q4" s="5163" t="n">
         <v>8.0</v>
       </c>
-      <c r="R4" s="5170"/>
+      <c r="R4" s="5167" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S4" s="5174"/>
       <c r="T4" s="5178"/>
       <c r="U4" s="5182"/>
@@ -6904,7 +6656,9 @@
       <c r="Q5" s="5287" t="n">
         <v>8.0</v>
       </c>
-      <c r="R5" s="5294"/>
+      <c r="R5" s="5291" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S5" s="5298"/>
       <c r="T5" s="5302"/>
       <c r="U5" s="5306"/>
@@ -6952,7 +6706,9 @@
       <c r="Q6" s="5411" t="n">
         <v>8.0</v>
       </c>
-      <c r="R6" s="5418"/>
+      <c r="R6" s="5415" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S6" s="5422"/>
       <c r="T6" s="5426"/>
       <c r="U6" s="5430"/>
@@ -7000,7 +6756,9 @@
       <c r="Q7" s="5535" t="n">
         <v>8.0</v>
       </c>
-      <c r="R7" s="5542"/>
+      <c r="R7" s="5539" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S7" s="5546"/>
       <c r="T7" s="5550"/>
       <c r="U7" s="5554"/>
@@ -7048,7 +6806,9 @@
       <c r="Q8" s="5659" t="n">
         <v>8.0</v>
       </c>
-      <c r="R8" s="5666"/>
+      <c r="R8" s="5663" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S8" s="5670"/>
       <c r="T8" s="5674"/>
       <c r="U8" s="5678"/>
@@ -7096,7 +6856,9 @@
       <c r="Q9" s="5783" t="n">
         <v>8.0</v>
       </c>
-      <c r="R9" s="5790"/>
+      <c r="R9" s="5787" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S9" s="5794"/>
       <c r="T9" s="5798"/>
       <c r="U9" s="5802"/>
@@ -7120,7 +6882,7 @@
       </c>
       <c r="B10" s="922" t="inlineStr">
         <is>
-          <t>Голод Иван Евгеньевич</t>
+          <t>Губайдулин Вадим Ринатович</t>
         </is>
       </c>
       <c r="C10" s="5854"/>
@@ -7144,7 +6906,9 @@
       <c r="Q10" s="5907" t="n">
         <v>8.0</v>
       </c>
-      <c r="R10" s="5914"/>
+      <c r="R10" s="5911" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S10" s="5918"/>
       <c r="T10" s="5922"/>
       <c r="U10" s="5926"/>
@@ -7168,7 +6932,7 @@
       </c>
       <c r="B11" s="1024" t="inlineStr">
         <is>
-          <t>Губайдулин Вадим Ринатович</t>
+          <t>Даниленко Никита Геннадьевич</t>
         </is>
       </c>
       <c r="C11" s="5978"/>
@@ -7192,7 +6956,9 @@
       <c r="Q11" s="6031" t="n">
         <v>8.0</v>
       </c>
-      <c r="R11" s="6038"/>
+      <c r="R11" s="6035" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S11" s="6042"/>
       <c r="T11" s="6046"/>
       <c r="U11" s="6050"/>
@@ -7216,7 +6982,7 @@
       </c>
       <c r="B12" s="1126" t="inlineStr">
         <is>
-          <t>Даниленко Никита Геннадьевич</t>
+          <t>Долгов Сергей Александрович</t>
         </is>
       </c>
       <c r="C12" s="6102"/>
@@ -7240,7 +7006,9 @@
       <c r="Q12" s="6155" t="n">
         <v>8.0</v>
       </c>
-      <c r="R12" s="6162"/>
+      <c r="R12" s="6159" t="n">
+        <v>8.0</v>
+      </c>
       <c r="S12" s="6166"/>
       <c r="T12" s="6170"/>
       <c r="U12" s="6174"/>
@@ -7259,99 +7027,75 @@
       <c r="AH12" s="1222"/>
     </row>
     <row r="13">
-      <c r="A13" s="1225" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B13" s="1228" t="inlineStr">
-        <is>
-          <t>Долгов Сергей Александрович</t>
-        </is>
-      </c>
-      <c r="C13" s="6226"/>
-      <c r="D13" s="6230"/>
-      <c r="E13" s="6234"/>
-      <c r="F13" s="6238"/>
-      <c r="G13" s="6242"/>
-      <c r="H13" s="6246"/>
-      <c r="I13" s="6250"/>
-      <c r="J13" s="6254"/>
-      <c r="K13" s="6258"/>
-      <c r="L13" s="6262"/>
-      <c r="M13" s="6266"/>
-      <c r="N13" s="6270"/>
-      <c r="O13" s="6271" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="P13" s="6275" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Q13" s="6279" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="R13" s="6286"/>
-      <c r="S13" s="6290"/>
-      <c r="T13" s="6294"/>
-      <c r="U13" s="6298"/>
-      <c r="V13" s="6302"/>
-      <c r="W13" s="6306"/>
-      <c r="X13" s="6310"/>
-      <c r="Y13" s="6314"/>
-      <c r="Z13" s="6318"/>
-      <c r="AA13" s="6322"/>
-      <c r="AB13" s="6326"/>
-      <c r="AC13" s="6330"/>
-      <c r="AD13" s="6334"/>
-      <c r="AE13" s="6338"/>
-      <c r="AF13" s="6342"/>
-      <c r="AG13" s="6346"/>
+      <c r="A13" s="1225"/>
+      <c r="B13" s="1228"/>
+      <c r="C13" s="1231"/>
+      <c r="D13" s="1234"/>
+      <c r="E13" s="1237"/>
+      <c r="F13" s="1240"/>
+      <c r="G13" s="1243"/>
+      <c r="H13" s="1246"/>
+      <c r="I13" s="1249"/>
+      <c r="J13" s="1252"/>
+      <c r="K13" s="1255"/>
+      <c r="L13" s="1258"/>
+      <c r="M13" s="1261"/>
+      <c r="N13" s="1264"/>
+      <c r="O13" s="1267"/>
+      <c r="P13" s="1270"/>
+      <c r="Q13" s="1273"/>
+      <c r="R13" s="1276"/>
+      <c r="S13" s="1279"/>
+      <c r="T13" s="1282"/>
+      <c r="U13" s="1285"/>
+      <c r="V13" s="1288"/>
+      <c r="W13" s="1291"/>
+      <c r="X13" s="1294"/>
+      <c r="Y13" s="1297"/>
+      <c r="Z13" s="1300"/>
+      <c r="AA13" s="1303"/>
+      <c r="AB13" s="1306"/>
+      <c r="AC13" s="1309"/>
+      <c r="AD13" s="1312"/>
+      <c r="AE13" s="1315"/>
+      <c r="AF13" s="1318"/>
+      <c r="AG13" s="1321"/>
       <c r="AH13" s="1324"/>
     </row>
     <row r="14">
-      <c r="A14" s="1327" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B14" s="1330" t="inlineStr">
-        <is>
-          <t>Дугаева Мария Николаевна</t>
-        </is>
-      </c>
-      <c r="C14" s="6350"/>
-      <c r="D14" s="6354"/>
-      <c r="E14" s="6358"/>
-      <c r="F14" s="6362"/>
-      <c r="G14" s="6366"/>
-      <c r="H14" s="6370"/>
-      <c r="I14" s="6374"/>
-      <c r="J14" s="6378"/>
-      <c r="K14" s="6382"/>
-      <c r="L14" s="6386"/>
-      <c r="M14" s="6390"/>
-      <c r="N14" s="6394"/>
-      <c r="O14" s="6395" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="P14" s="6399" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="Q14" s="6403" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="R14" s="6410"/>
-      <c r="S14" s="6414"/>
-      <c r="T14" s="6418"/>
-      <c r="U14" s="6422"/>
-      <c r="V14" s="6426"/>
-      <c r="W14" s="6430"/>
-      <c r="X14" s="6434"/>
-      <c r="Y14" s="6438"/>
-      <c r="Z14" s="6442"/>
-      <c r="AA14" s="6446"/>
-      <c r="AB14" s="6450"/>
-      <c r="AC14" s="6454"/>
-      <c r="AD14" s="6458"/>
-      <c r="AE14" s="6462"/>
-      <c r="AF14" s="6466"/>
-      <c r="AG14" s="6470"/>
+      <c r="A14" s="1327"/>
+      <c r="B14" s="1330"/>
+      <c r="C14" s="1333"/>
+      <c r="D14" s="1336"/>
+      <c r="E14" s="1339"/>
+      <c r="F14" s="1342"/>
+      <c r="G14" s="1345"/>
+      <c r="H14" s="1348"/>
+      <c r="I14" s="1351"/>
+      <c r="J14" s="1354"/>
+      <c r="K14" s="1357"/>
+      <c r="L14" s="1360"/>
+      <c r="M14" s="1363"/>
+      <c r="N14" s="1366"/>
+      <c r="O14" s="1369"/>
+      <c r="P14" s="1372"/>
+      <c r="Q14" s="1375"/>
+      <c r="R14" s="1378"/>
+      <c r="S14" s="1381"/>
+      <c r="T14" s="1384"/>
+      <c r="U14" s="1387"/>
+      <c r="V14" s="1390"/>
+      <c r="W14" s="1393"/>
+      <c r="X14" s="1396"/>
+      <c r="Y14" s="1399"/>
+      <c r="Z14" s="1402"/>
+      <c r="AA14" s="1405"/>
+      <c r="AB14" s="1408"/>
+      <c r="AC14" s="1411"/>
+      <c r="AD14" s="1414"/>
+      <c r="AE14" s="1417"/>
+      <c r="AF14" s="1420"/>
+      <c r="AG14" s="1423"/>
       <c r="AH14" s="1426"/>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Begin reorganize workers. Split to some massive. Complete reports of months
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -2983,8 +2983,10 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="1701" t="n">
-        <v>1.0</v>
+      <c r="C1" s="1701" t="inlineStr">
+        <is>
+          <t>Июль</t>
+        </is>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
@@ -3181,10 +3183,10 @@
       <c r="L4" s="1742"/>
       <c r="M4" s="1746"/>
       <c r="N4" s="1750"/>
-      <c r="O4" s="1751"/>
-      <c r="P4" s="1757"/>
-      <c r="Q4" s="1759"/>
-      <c r="R4" s="1763"/>
+      <c r="O4" s="1754"/>
+      <c r="P4" s="1758"/>
+      <c r="Q4" s="1762"/>
+      <c r="R4" s="1766"/>
       <c r="S4" s="1770"/>
       <c r="T4" s="1774"/>
       <c r="U4" s="1778"/>
@@ -3199,7 +3201,9 @@
       <c r="AD4" s="1814"/>
       <c r="AE4" s="1818"/>
       <c r="AF4" s="1822"/>
-      <c r="AG4" s="1826"/>
+      <c r="AG4" s="1823" t="n">
+        <v>8.0</v>
+      </c>
       <c r="AH4" s="136"/>
     </row>
     <row r="5">
@@ -3223,10 +3227,10 @@
       <c r="L5" s="1866"/>
       <c r="M5" s="1870"/>
       <c r="N5" s="1874"/>
-      <c r="O5" s="1877"/>
-      <c r="P5" s="1881"/>
-      <c r="Q5" s="1883"/>
-      <c r="R5" s="1887"/>
+      <c r="O5" s="1878"/>
+      <c r="P5" s="1882"/>
+      <c r="Q5" s="1886"/>
+      <c r="R5" s="1890"/>
       <c r="S5" s="1894"/>
       <c r="T5" s="1898"/>
       <c r="U5" s="1902"/>
@@ -3241,7 +3245,9 @@
       <c r="AD5" s="1938"/>
       <c r="AE5" s="1942"/>
       <c r="AF5" s="1946"/>
-      <c r="AG5" s="1950"/>
+      <c r="AG5" s="1947" t="n">
+        <v>8.0</v>
+      </c>
       <c r="AH5" s="170"/>
     </row>
     <row r="6">
@@ -3265,10 +3271,10 @@
       <c r="L6" s="1990"/>
       <c r="M6" s="1994"/>
       <c r="N6" s="1998"/>
-      <c r="O6" s="1999"/>
-      <c r="P6" s="2003"/>
-      <c r="Q6" s="2007"/>
-      <c r="R6" s="2011"/>
+      <c r="O6" s="2002"/>
+      <c r="P6" s="2006"/>
+      <c r="Q6" s="2010"/>
+      <c r="R6" s="2014"/>
       <c r="S6" s="2018"/>
       <c r="T6" s="2022"/>
       <c r="U6" s="2026"/>
@@ -3283,7 +3289,7 @@
       <c r="AD6" s="2062"/>
       <c r="AE6" s="2066"/>
       <c r="AF6" s="2070"/>
-      <c r="AG6" s="2074"/>
+      <c r="AG6" s="2073"/>
       <c r="AH6" s="204"/>
     </row>
     <row r="7">
@@ -3307,10 +3313,10 @@
       <c r="L7" s="2114"/>
       <c r="M7" s="2118"/>
       <c r="N7" s="2122"/>
-      <c r="O7" s="2123"/>
-      <c r="P7" s="2127"/>
-      <c r="Q7" s="2131"/>
-      <c r="R7" s="2135"/>
+      <c r="O7" s="2126"/>
+      <c r="P7" s="2130"/>
+      <c r="Q7" s="2134"/>
+      <c r="R7" s="2138"/>
       <c r="S7" s="2142"/>
       <c r="T7" s="2146"/>
       <c r="U7" s="2150"/>
@@ -3325,7 +3331,7 @@
       <c r="AD7" s="2186"/>
       <c r="AE7" s="2190"/>
       <c r="AF7" s="2194"/>
-      <c r="AG7" s="2198"/>
+      <c r="AG7" s="2196"/>
       <c r="AH7" s="238"/>
     </row>
     <row r="8">
@@ -3349,10 +3355,10 @@
       <c r="L8" s="2238"/>
       <c r="M8" s="2242"/>
       <c r="N8" s="2246"/>
-      <c r="O8" s="2247"/>
-      <c r="P8" s="2251"/>
-      <c r="Q8" s="2255"/>
-      <c r="R8" s="2259"/>
+      <c r="O8" s="2250"/>
+      <c r="P8" s="2254"/>
+      <c r="Q8" s="2258"/>
+      <c r="R8" s="2262"/>
       <c r="S8" s="2266"/>
       <c r="T8" s="2270"/>
       <c r="U8" s="2274"/>
@@ -3367,7 +3373,7 @@
       <c r="AD8" s="2310"/>
       <c r="AE8" s="2314"/>
       <c r="AF8" s="2318"/>
-      <c r="AG8" s="2322"/>
+      <c r="AG8" s="2320"/>
       <c r="AH8" s="272"/>
     </row>
     <row r="9">
@@ -3391,10 +3397,10 @@
       <c r="L9" s="2362"/>
       <c r="M9" s="2366"/>
       <c r="N9" s="2370"/>
-      <c r="O9" s="2371"/>
-      <c r="P9" s="2375"/>
-      <c r="Q9" s="2379"/>
-      <c r="R9" s="2383"/>
+      <c r="O9" s="2374"/>
+      <c r="P9" s="2378"/>
+      <c r="Q9" s="2382"/>
+      <c r="R9" s="2386"/>
       <c r="S9" s="2390"/>
       <c r="T9" s="2394"/>
       <c r="U9" s="2398"/>
@@ -3433,10 +3439,10 @@
       <c r="L10" s="2486"/>
       <c r="M10" s="2490"/>
       <c r="N10" s="2494"/>
-      <c r="O10" s="2495"/>
-      <c r="P10" s="2499"/>
-      <c r="Q10" s="2503"/>
-      <c r="R10" s="2507"/>
+      <c r="O10" s="2498"/>
+      <c r="P10" s="2502"/>
+      <c r="Q10" s="2506"/>
+      <c r="R10" s="2510"/>
       <c r="S10" s="2514"/>
       <c r="T10" s="2518"/>
       <c r="U10" s="2522"/>
@@ -3451,7 +3457,9 @@
       <c r="AD10" s="2558"/>
       <c r="AE10" s="2562"/>
       <c r="AF10" s="2566"/>
-      <c r="AG10" s="2570"/>
+      <c r="AG10" s="2567" t="n">
+        <v>3.0</v>
+      </c>
       <c r="AH10" s="340"/>
     </row>
     <row r="11">
@@ -3475,10 +3483,10 @@
       <c r="L11" s="2610"/>
       <c r="M11" s="2614"/>
       <c r="N11" s="2618"/>
-      <c r="O11" s="2619"/>
-      <c r="P11" s="2623"/>
-      <c r="Q11" s="2627"/>
-      <c r="R11" s="2631"/>
+      <c r="O11" s="2622"/>
+      <c r="P11" s="2626"/>
+      <c r="Q11" s="2630"/>
+      <c r="R11" s="2634"/>
       <c r="S11" s="2638"/>
       <c r="T11" s="2642"/>
       <c r="U11" s="2646"/>
@@ -3493,7 +3501,9 @@
       <c r="AD11" s="2682"/>
       <c r="AE11" s="2686"/>
       <c r="AF11" s="2690"/>
-      <c r="AG11" s="2694"/>
+      <c r="AG11" s="2691" t="n">
+        <v>8.0</v>
+      </c>
       <c r="AH11" s="374"/>
     </row>
     <row r="12">
@@ -3517,10 +3527,10 @@
       <c r="L12" s="2734"/>
       <c r="M12" s="2738"/>
       <c r="N12" s="2742"/>
-      <c r="O12" s="2743"/>
-      <c r="P12" s="2747"/>
-      <c r="Q12" s="2751"/>
-      <c r="R12" s="2755"/>
+      <c r="O12" s="2746"/>
+      <c r="P12" s="2750"/>
+      <c r="Q12" s="2754"/>
+      <c r="R12" s="2758"/>
       <c r="S12" s="2762"/>
       <c r="T12" s="2766"/>
       <c r="U12" s="2770"/>
@@ -3535,7 +3545,9 @@
       <c r="AD12" s="2806"/>
       <c r="AE12" s="2810"/>
       <c r="AF12" s="2814"/>
-      <c r="AG12" s="2818"/>
+      <c r="AG12" s="2815" t="n">
+        <v>1.0</v>
+      </c>
       <c r="AH12" s="408"/>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
reorganize some logic in GridEdit.java
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Бригада техники" r:id="rId3" sheetId="1"/>
+    <sheet name="Бригада сборщики" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2819">
+  <cellXfs count="1827">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -1816,998 +1816,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
@@ -2985,7 +1993,7 @@
       <c r="B1" s="2"/>
       <c r="C1" s="1701" t="inlineStr">
         <is>
-          <t>Июль</t>
+          <t>Август</t>
         </is>
       </c>
       <c r="D1" s="4"/>
@@ -3168,7 +2176,7 @@
       </c>
       <c r="B4" s="104" t="inlineStr">
         <is>
-          <t>Паньков Евгений Олегович</t>
+          <t>Петров Петр Петрович</t>
         </is>
       </c>
       <c r="C4" s="1706"/>
@@ -3186,7 +2194,7 @@
       <c r="O4" s="1754"/>
       <c r="P4" s="1758"/>
       <c r="Q4" s="1762"/>
-      <c r="R4" s="1766"/>
+      <c r="R4" s="1765"/>
       <c r="S4" s="1770"/>
       <c r="T4" s="1774"/>
       <c r="U4" s="1778"/>
@@ -3201,353 +2209,295 @@
       <c r="AD4" s="1814"/>
       <c r="AE4" s="1818"/>
       <c r="AF4" s="1822"/>
-      <c r="AG4" s="1823" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="AG4" s="1826"/>
       <c r="AH4" s="136"/>
     </row>
     <row r="5">
-      <c r="A5" s="137" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B5" s="138" t="inlineStr">
-        <is>
-          <t>Марков Евгений Викторович</t>
-        </is>
-      </c>
-      <c r="C5" s="1830"/>
-      <c r="D5" s="1834"/>
-      <c r="E5" s="1838"/>
-      <c r="F5" s="1842"/>
-      <c r="G5" s="1846"/>
-      <c r="H5" s="1850"/>
-      <c r="I5" s="1854"/>
-      <c r="J5" s="1858"/>
-      <c r="K5" s="1862"/>
-      <c r="L5" s="1866"/>
-      <c r="M5" s="1870"/>
-      <c r="N5" s="1874"/>
-      <c r="O5" s="1878"/>
-      <c r="P5" s="1882"/>
-      <c r="Q5" s="1886"/>
-      <c r="R5" s="1890"/>
-      <c r="S5" s="1894"/>
-      <c r="T5" s="1898"/>
-      <c r="U5" s="1902"/>
-      <c r="V5" s="1906"/>
-      <c r="W5" s="1910"/>
-      <c r="X5" s="1914"/>
-      <c r="Y5" s="1918"/>
-      <c r="Z5" s="1922"/>
-      <c r="AA5" s="1926"/>
-      <c r="AB5" s="1930"/>
-      <c r="AC5" s="1934"/>
-      <c r="AD5" s="1938"/>
-      <c r="AE5" s="1942"/>
-      <c r="AF5" s="1946"/>
-      <c r="AG5" s="1947" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="A5" s="137"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="148"/>
+      <c r="M5" s="149"/>
+      <c r="N5" s="150"/>
+      <c r="O5" s="151"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="153"/>
+      <c r="R5" s="154"/>
+      <c r="S5" s="155"/>
+      <c r="T5" s="156"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="158"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="160"/>
+      <c r="Y5" s="161"/>
+      <c r="Z5" s="162"/>
+      <c r="AA5" s="163"/>
+      <c r="AB5" s="164"/>
+      <c r="AC5" s="165"/>
+      <c r="AD5" s="166"/>
+      <c r="AE5" s="167"/>
+      <c r="AF5" s="168"/>
+      <c r="AG5" s="169"/>
       <c r="AH5" s="170"/>
     </row>
     <row r="6">
-      <c r="A6" s="171" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B6" s="172" t="inlineStr">
-        <is>
-          <t>Слегин Руслан Игоревич</t>
-        </is>
-      </c>
-      <c r="C6" s="1954"/>
-      <c r="D6" s="1958"/>
-      <c r="E6" s="1962"/>
-      <c r="F6" s="1966"/>
-      <c r="G6" s="1970"/>
-      <c r="H6" s="1974"/>
-      <c r="I6" s="1978"/>
-      <c r="J6" s="1982"/>
-      <c r="K6" s="1986"/>
-      <c r="L6" s="1990"/>
-      <c r="M6" s="1994"/>
-      <c r="N6" s="1998"/>
-      <c r="O6" s="2002"/>
-      <c r="P6" s="2006"/>
-      <c r="Q6" s="2010"/>
-      <c r="R6" s="2014"/>
-      <c r="S6" s="2018"/>
-      <c r="T6" s="2022"/>
-      <c r="U6" s="2026"/>
-      <c r="V6" s="2030"/>
-      <c r="W6" s="2034"/>
-      <c r="X6" s="2038"/>
-      <c r="Y6" s="2042"/>
-      <c r="Z6" s="2046"/>
-      <c r="AA6" s="2050"/>
-      <c r="AB6" s="2054"/>
-      <c r="AC6" s="2058"/>
-      <c r="AD6" s="2062"/>
-      <c r="AE6" s="2066"/>
-      <c r="AF6" s="2070"/>
-      <c r="AG6" s="2073"/>
+      <c r="A6" s="171"/>
+      <c r="B6" s="172"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="180"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="182"/>
+      <c r="M6" s="183"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="185"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="188"/>
+      <c r="S6" s="189"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="191"/>
+      <c r="V6" s="192"/>
+      <c r="W6" s="193"/>
+      <c r="X6" s="194"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="196"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="198"/>
+      <c r="AC6" s="199"/>
+      <c r="AD6" s="200"/>
+      <c r="AE6" s="201"/>
+      <c r="AF6" s="202"/>
+      <c r="AG6" s="203"/>
       <c r="AH6" s="204"/>
     </row>
     <row r="7">
-      <c r="A7" s="205" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="206" t="inlineStr">
-        <is>
-          <t>Зуев Сергей Константинович</t>
-        </is>
-      </c>
-      <c r="C7" s="2078"/>
-      <c r="D7" s="2082"/>
-      <c r="E7" s="2086"/>
-      <c r="F7" s="2090"/>
-      <c r="G7" s="2094"/>
-      <c r="H7" s="2098"/>
-      <c r="I7" s="2102"/>
-      <c r="J7" s="2106"/>
-      <c r="K7" s="2110"/>
-      <c r="L7" s="2114"/>
-      <c r="M7" s="2118"/>
-      <c r="N7" s="2122"/>
-      <c r="O7" s="2126"/>
-      <c r="P7" s="2130"/>
-      <c r="Q7" s="2134"/>
-      <c r="R7" s="2138"/>
-      <c r="S7" s="2142"/>
-      <c r="T7" s="2146"/>
-      <c r="U7" s="2150"/>
-      <c r="V7" s="2154"/>
-      <c r="W7" s="2158"/>
-      <c r="X7" s="2162"/>
-      <c r="Y7" s="2166"/>
-      <c r="Z7" s="2170"/>
-      <c r="AA7" s="2174"/>
-      <c r="AB7" s="2178"/>
-      <c r="AC7" s="2182"/>
-      <c r="AD7" s="2186"/>
-      <c r="AE7" s="2190"/>
-      <c r="AF7" s="2194"/>
-      <c r="AG7" s="2196"/>
+      <c r="A7" s="205"/>
+      <c r="B7" s="206"/>
+      <c r="C7" s="207"/>
+      <c r="D7" s="208"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="210"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="212"/>
+      <c r="I7" s="213"/>
+      <c r="J7" s="214"/>
+      <c r="K7" s="215"/>
+      <c r="L7" s="216"/>
+      <c r="M7" s="217"/>
+      <c r="N7" s="218"/>
+      <c r="O7" s="219"/>
+      <c r="P7" s="220"/>
+      <c r="Q7" s="221"/>
+      <c r="R7" s="222"/>
+      <c r="S7" s="223"/>
+      <c r="T7" s="224"/>
+      <c r="U7" s="225"/>
+      <c r="V7" s="226"/>
+      <c r="W7" s="227"/>
+      <c r="X7" s="228"/>
+      <c r="Y7" s="229"/>
+      <c r="Z7" s="230"/>
+      <c r="AA7" s="231"/>
+      <c r="AB7" s="232"/>
+      <c r="AC7" s="233"/>
+      <c r="AD7" s="234"/>
+      <c r="AE7" s="235"/>
+      <c r="AF7" s="236"/>
+      <c r="AG7" s="237"/>
       <c r="AH7" s="238"/>
     </row>
     <row r="8">
-      <c r="A8" s="239" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B8" s="240" t="inlineStr">
-        <is>
-          <t>Абенд Евгений Сергеевич</t>
-        </is>
-      </c>
-      <c r="C8" s="2202"/>
-      <c r="D8" s="2206"/>
-      <c r="E8" s="2210"/>
-      <c r="F8" s="2214"/>
-      <c r="G8" s="2218"/>
-      <c r="H8" s="2222"/>
-      <c r="I8" s="2226"/>
-      <c r="J8" s="2230"/>
-      <c r="K8" s="2234"/>
-      <c r="L8" s="2238"/>
-      <c r="M8" s="2242"/>
-      <c r="N8" s="2246"/>
-      <c r="O8" s="2250"/>
-      <c r="P8" s="2254"/>
-      <c r="Q8" s="2258"/>
-      <c r="R8" s="2262"/>
-      <c r="S8" s="2266"/>
-      <c r="T8" s="2270"/>
-      <c r="U8" s="2274"/>
-      <c r="V8" s="2278"/>
-      <c r="W8" s="2282"/>
-      <c r="X8" s="2286"/>
-      <c r="Y8" s="2290"/>
-      <c r="Z8" s="2294"/>
-      <c r="AA8" s="2298"/>
-      <c r="AB8" s="2302"/>
-      <c r="AC8" s="2306"/>
-      <c r="AD8" s="2310"/>
-      <c r="AE8" s="2314"/>
-      <c r="AF8" s="2318"/>
-      <c r="AG8" s="2320"/>
+      <c r="A8" s="239"/>
+      <c r="B8" s="240"/>
+      <c r="C8" s="241"/>
+      <c r="D8" s="242"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="246"/>
+      <c r="I8" s="247"/>
+      <c r="J8" s="248"/>
+      <c r="K8" s="249"/>
+      <c r="L8" s="250"/>
+      <c r="M8" s="251"/>
+      <c r="N8" s="252"/>
+      <c r="O8" s="253"/>
+      <c r="P8" s="254"/>
+      <c r="Q8" s="255"/>
+      <c r="R8" s="256"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="259"/>
+      <c r="V8" s="260"/>
+      <c r="W8" s="261"/>
+      <c r="X8" s="262"/>
+      <c r="Y8" s="263"/>
+      <c r="Z8" s="264"/>
+      <c r="AA8" s="265"/>
+      <c r="AB8" s="266"/>
+      <c r="AC8" s="267"/>
+      <c r="AD8" s="268"/>
+      <c r="AE8" s="269"/>
+      <c r="AF8" s="270"/>
+      <c r="AG8" s="271"/>
       <c r="AH8" s="272"/>
     </row>
     <row r="9">
-      <c r="A9" s="273" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="274" t="inlineStr">
-        <is>
-          <t>Болгаров Вениамин Владимирович</t>
-        </is>
-      </c>
-      <c r="C9" s="2326"/>
-      <c r="D9" s="2330"/>
-      <c r="E9" s="2334"/>
-      <c r="F9" s="2338"/>
-      <c r="G9" s="2342"/>
-      <c r="H9" s="2346"/>
-      <c r="I9" s="2350"/>
-      <c r="J9" s="2354"/>
-      <c r="K9" s="2358"/>
-      <c r="L9" s="2362"/>
-      <c r="M9" s="2366"/>
-      <c r="N9" s="2370"/>
-      <c r="O9" s="2374"/>
-      <c r="P9" s="2378"/>
-      <c r="Q9" s="2382"/>
-      <c r="R9" s="2386"/>
-      <c r="S9" s="2390"/>
-      <c r="T9" s="2394"/>
-      <c r="U9" s="2398"/>
-      <c r="V9" s="2402"/>
-      <c r="W9" s="2406"/>
-      <c r="X9" s="2410"/>
-      <c r="Y9" s="2414"/>
-      <c r="Z9" s="2418"/>
-      <c r="AA9" s="2422"/>
-      <c r="AB9" s="2426"/>
-      <c r="AC9" s="2430"/>
-      <c r="AD9" s="2434"/>
-      <c r="AE9" s="2438"/>
-      <c r="AF9" s="2442"/>
-      <c r="AG9" s="2446"/>
+      <c r="A9" s="273"/>
+      <c r="B9" s="274"/>
+      <c r="C9" s="275"/>
+      <c r="D9" s="276"/>
+      <c r="E9" s="277"/>
+      <c r="F9" s="278"/>
+      <c r="G9" s="279"/>
+      <c r="H9" s="280"/>
+      <c r="I9" s="281"/>
+      <c r="J9" s="282"/>
+      <c r="K9" s="283"/>
+      <c r="L9" s="284"/>
+      <c r="M9" s="285"/>
+      <c r="N9" s="286"/>
+      <c r="O9" s="287"/>
+      <c r="P9" s="288"/>
+      <c r="Q9" s="289"/>
+      <c r="R9" s="290"/>
+      <c r="S9" s="291"/>
+      <c r="T9" s="292"/>
+      <c r="U9" s="293"/>
+      <c r="V9" s="294"/>
+      <c r="W9" s="295"/>
+      <c r="X9" s="296"/>
+      <c r="Y9" s="297"/>
+      <c r="Z9" s="298"/>
+      <c r="AA9" s="299"/>
+      <c r="AB9" s="300"/>
+      <c r="AC9" s="301"/>
+      <c r="AD9" s="302"/>
+      <c r="AE9" s="303"/>
+      <c r="AF9" s="304"/>
+      <c r="AG9" s="305"/>
       <c r="AH9" s="306"/>
     </row>
     <row r="10">
-      <c r="A10" s="307" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B10" s="308" t="inlineStr">
-        <is>
-          <t>Губайдулин Вадим Ринатович</t>
-        </is>
-      </c>
-      <c r="C10" s="2450"/>
-      <c r="D10" s="2454"/>
-      <c r="E10" s="2458"/>
-      <c r="F10" s="2462"/>
-      <c r="G10" s="2466"/>
-      <c r="H10" s="2470"/>
-      <c r="I10" s="2474"/>
-      <c r="J10" s="2478"/>
-      <c r="K10" s="2482"/>
-      <c r="L10" s="2486"/>
-      <c r="M10" s="2490"/>
-      <c r="N10" s="2494"/>
-      <c r="O10" s="2498"/>
-      <c r="P10" s="2502"/>
-      <c r="Q10" s="2506"/>
-      <c r="R10" s="2510"/>
-      <c r="S10" s="2514"/>
-      <c r="T10" s="2518"/>
-      <c r="U10" s="2522"/>
-      <c r="V10" s="2526"/>
-      <c r="W10" s="2530"/>
-      <c r="X10" s="2534"/>
-      <c r="Y10" s="2538"/>
-      <c r="Z10" s="2542"/>
-      <c r="AA10" s="2546"/>
-      <c r="AB10" s="2550"/>
-      <c r="AC10" s="2554"/>
-      <c r="AD10" s="2558"/>
-      <c r="AE10" s="2562"/>
-      <c r="AF10" s="2566"/>
-      <c r="AG10" s="2567" t="n">
-        <v>3.0</v>
-      </c>
+      <c r="A10" s="307"/>
+      <c r="B10" s="308"/>
+      <c r="C10" s="309"/>
+      <c r="D10" s="310"/>
+      <c r="E10" s="311"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="313"/>
+      <c r="H10" s="314"/>
+      <c r="I10" s="315"/>
+      <c r="J10" s="316"/>
+      <c r="K10" s="317"/>
+      <c r="L10" s="318"/>
+      <c r="M10" s="319"/>
+      <c r="N10" s="320"/>
+      <c r="O10" s="321"/>
+      <c r="P10" s="322"/>
+      <c r="Q10" s="323"/>
+      <c r="R10" s="324"/>
+      <c r="S10" s="325"/>
+      <c r="T10" s="326"/>
+      <c r="U10" s="327"/>
+      <c r="V10" s="328"/>
+      <c r="W10" s="329"/>
+      <c r="X10" s="330"/>
+      <c r="Y10" s="331"/>
+      <c r="Z10" s="332"/>
+      <c r="AA10" s="333"/>
+      <c r="AB10" s="334"/>
+      <c r="AC10" s="335"/>
+      <c r="AD10" s="336"/>
+      <c r="AE10" s="337"/>
+      <c r="AF10" s="338"/>
+      <c r="AG10" s="339"/>
       <c r="AH10" s="340"/>
     </row>
     <row r="11">
-      <c r="A11" s="341" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B11" s="342" t="inlineStr">
-        <is>
-          <t>Даниленко Никита Геннадьевич</t>
-        </is>
-      </c>
-      <c r="C11" s="2574"/>
-      <c r="D11" s="2578"/>
-      <c r="E11" s="2582"/>
-      <c r="F11" s="2586"/>
-      <c r="G11" s="2590"/>
-      <c r="H11" s="2594"/>
-      <c r="I11" s="2598"/>
-      <c r="J11" s="2602"/>
-      <c r="K11" s="2606"/>
-      <c r="L11" s="2610"/>
-      <c r="M11" s="2614"/>
-      <c r="N11" s="2618"/>
-      <c r="O11" s="2622"/>
-      <c r="P11" s="2626"/>
-      <c r="Q11" s="2630"/>
-      <c r="R11" s="2634"/>
-      <c r="S11" s="2638"/>
-      <c r="T11" s="2642"/>
-      <c r="U11" s="2646"/>
-      <c r="V11" s="2650"/>
-      <c r="W11" s="2654"/>
-      <c r="X11" s="2658"/>
-      <c r="Y11" s="2662"/>
-      <c r="Z11" s="2666"/>
-      <c r="AA11" s="2670"/>
-      <c r="AB11" s="2674"/>
-      <c r="AC11" s="2678"/>
-      <c r="AD11" s="2682"/>
-      <c r="AE11" s="2686"/>
-      <c r="AF11" s="2690"/>
-      <c r="AG11" s="2691" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="A11" s="341"/>
+      <c r="B11" s="342"/>
+      <c r="C11" s="343"/>
+      <c r="D11" s="344"/>
+      <c r="E11" s="345"/>
+      <c r="F11" s="346"/>
+      <c r="G11" s="347"/>
+      <c r="H11" s="348"/>
+      <c r="I11" s="349"/>
+      <c r="J11" s="350"/>
+      <c r="K11" s="351"/>
+      <c r="L11" s="352"/>
+      <c r="M11" s="353"/>
+      <c r="N11" s="354"/>
+      <c r="O11" s="355"/>
+      <c r="P11" s="356"/>
+      <c r="Q11" s="357"/>
+      <c r="R11" s="358"/>
+      <c r="S11" s="359"/>
+      <c r="T11" s="360"/>
+      <c r="U11" s="361"/>
+      <c r="V11" s="362"/>
+      <c r="W11" s="363"/>
+      <c r="X11" s="364"/>
+      <c r="Y11" s="365"/>
+      <c r="Z11" s="366"/>
+      <c r="AA11" s="367"/>
+      <c r="AB11" s="368"/>
+      <c r="AC11" s="369"/>
+      <c r="AD11" s="370"/>
+      <c r="AE11" s="371"/>
+      <c r="AF11" s="372"/>
+      <c r="AG11" s="373"/>
       <c r="AH11" s="374"/>
     </row>
     <row r="12">
-      <c r="A12" s="375" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B12" s="376" t="inlineStr">
-        <is>
-          <t>Долгов Сергей Александрович</t>
-        </is>
-      </c>
-      <c r="C12" s="2698"/>
-      <c r="D12" s="2702"/>
-      <c r="E12" s="2706"/>
-      <c r="F12" s="2710"/>
-      <c r="G12" s="2714"/>
-      <c r="H12" s="2718"/>
-      <c r="I12" s="2722"/>
-      <c r="J12" s="2726"/>
-      <c r="K12" s="2730"/>
-      <c r="L12" s="2734"/>
-      <c r="M12" s="2738"/>
-      <c r="N12" s="2742"/>
-      <c r="O12" s="2746"/>
-      <c r="P12" s="2750"/>
-      <c r="Q12" s="2754"/>
-      <c r="R12" s="2758"/>
-      <c r="S12" s="2762"/>
-      <c r="T12" s="2766"/>
-      <c r="U12" s="2770"/>
-      <c r="V12" s="2774"/>
-      <c r="W12" s="2778"/>
-      <c r="X12" s="2782"/>
-      <c r="Y12" s="2786"/>
-      <c r="Z12" s="2790"/>
-      <c r="AA12" s="2794"/>
-      <c r="AB12" s="2798"/>
-      <c r="AC12" s="2802"/>
-      <c r="AD12" s="2806"/>
-      <c r="AE12" s="2810"/>
-      <c r="AF12" s="2814"/>
-      <c r="AG12" s="2815" t="n">
-        <v>1.0</v>
-      </c>
+      <c r="A12" s="375"/>
+      <c r="B12" s="376"/>
+      <c r="C12" s="377"/>
+      <c r="D12" s="378"/>
+      <c r="E12" s="379"/>
+      <c r="F12" s="380"/>
+      <c r="G12" s="381"/>
+      <c r="H12" s="382"/>
+      <c r="I12" s="383"/>
+      <c r="J12" s="384"/>
+      <c r="K12" s="385"/>
+      <c r="L12" s="386"/>
+      <c r="M12" s="387"/>
+      <c r="N12" s="388"/>
+      <c r="O12" s="389"/>
+      <c r="P12" s="390"/>
+      <c r="Q12" s="391"/>
+      <c r="R12" s="392"/>
+      <c r="S12" s="393"/>
+      <c r="T12" s="394"/>
+      <c r="U12" s="395"/>
+      <c r="V12" s="396"/>
+      <c r="W12" s="397"/>
+      <c r="X12" s="398"/>
+      <c r="Y12" s="399"/>
+      <c r="Z12" s="400"/>
+      <c r="AA12" s="401"/>
+      <c r="AB12" s="402"/>
+      <c r="AC12" s="403"/>
+      <c r="AD12" s="404"/>
+      <c r="AE12" s="405"/>
+      <c r="AF12" s="406"/>
+      <c r="AG12" s="407"/>
       <c r="AH12" s="408"/>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
new split to line for workers
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2819">
+  <cellXfs count="1827">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
@@ -1816,998 +1816,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true"/>
@@ -2985,7 +1993,7 @@
       <c r="B1" s="2"/>
       <c r="C1" s="1701" t="inlineStr">
         <is>
-          <t>Январь</t>
+          <t>Август</t>
         </is>
       </c>
       <c r="D1" s="4"/>
@@ -3168,7 +2176,7 @@
       </c>
       <c r="B4" s="104" t="inlineStr">
         <is>
-          <t>Паньков Евгений Олегович</t>
+          <t>Марков Евгений Викторович</t>
         </is>
       </c>
       <c r="C4" s="1706"/>
@@ -3205,339 +2213,291 @@
       <c r="AH4" s="136"/>
     </row>
     <row r="5">
-      <c r="A5" s="137" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B5" s="138" t="inlineStr">
-        <is>
-          <t>Марков Евгений Викторович</t>
-        </is>
-      </c>
-      <c r="C5" s="1830"/>
-      <c r="D5" s="1834"/>
-      <c r="E5" s="1838"/>
-      <c r="F5" s="1842"/>
-      <c r="G5" s="1846"/>
-      <c r="H5" s="1850"/>
-      <c r="I5" s="1854"/>
-      <c r="J5" s="1858"/>
-      <c r="K5" s="1862"/>
-      <c r="L5" s="1866"/>
-      <c r="M5" s="1870"/>
-      <c r="N5" s="1874"/>
-      <c r="O5" s="1878"/>
-      <c r="P5" s="1882"/>
-      <c r="Q5" s="1886"/>
-      <c r="R5" s="1890"/>
-      <c r="S5" s="1894"/>
-      <c r="T5" s="1898"/>
-      <c r="U5" s="1902"/>
-      <c r="V5" s="1906"/>
-      <c r="W5" s="1910"/>
-      <c r="X5" s="1914"/>
-      <c r="Y5" s="1918"/>
-      <c r="Z5" s="1922"/>
-      <c r="AA5" s="1926"/>
-      <c r="AB5" s="1930"/>
-      <c r="AC5" s="1934"/>
-      <c r="AD5" s="1938"/>
-      <c r="AE5" s="1942"/>
-      <c r="AF5" s="1946"/>
-      <c r="AG5" s="1950"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="139"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="148"/>
+      <c r="M5" s="149"/>
+      <c r="N5" s="150"/>
+      <c r="O5" s="151"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="153"/>
+      <c r="R5" s="154"/>
+      <c r="S5" s="155"/>
+      <c r="T5" s="156"/>
+      <c r="U5" s="157"/>
+      <c r="V5" s="158"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="160"/>
+      <c r="Y5" s="161"/>
+      <c r="Z5" s="162"/>
+      <c r="AA5" s="163"/>
+      <c r="AB5" s="164"/>
+      <c r="AC5" s="165"/>
+      <c r="AD5" s="166"/>
+      <c r="AE5" s="167"/>
+      <c r="AF5" s="168"/>
+      <c r="AG5" s="169"/>
       <c r="AH5" s="170"/>
     </row>
     <row r="6">
-      <c r="A6" s="171" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B6" s="172" t="inlineStr">
-        <is>
-          <t>Слегин Руслан Игоревич</t>
-        </is>
-      </c>
-      <c r="C6" s="1954"/>
-      <c r="D6" s="1958"/>
-      <c r="E6" s="1962"/>
-      <c r="F6" s="1966"/>
-      <c r="G6" s="1970"/>
-      <c r="H6" s="1974"/>
-      <c r="I6" s="1978"/>
-      <c r="J6" s="1982"/>
-      <c r="K6" s="1986"/>
-      <c r="L6" s="1990"/>
-      <c r="M6" s="1994"/>
-      <c r="N6" s="1998"/>
-      <c r="O6" s="2002"/>
-      <c r="P6" s="2006"/>
-      <c r="Q6" s="2010"/>
-      <c r="R6" s="2014"/>
-      <c r="S6" s="2018"/>
-      <c r="T6" s="2022"/>
-      <c r="U6" s="2026"/>
-      <c r="V6" s="2030"/>
-      <c r="W6" s="2034"/>
-      <c r="X6" s="2038"/>
-      <c r="Y6" s="2042"/>
-      <c r="Z6" s="2046"/>
-      <c r="AA6" s="2050"/>
-      <c r="AB6" s="2054"/>
-      <c r="AC6" s="2058"/>
-      <c r="AD6" s="2062"/>
-      <c r="AE6" s="2066"/>
-      <c r="AF6" s="2070"/>
-      <c r="AG6" s="2074"/>
+      <c r="A6" s="171"/>
+      <c r="B6" s="172"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="174"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="178"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="180"/>
+      <c r="K6" s="181"/>
+      <c r="L6" s="182"/>
+      <c r="M6" s="183"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="185"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="188"/>
+      <c r="S6" s="189"/>
+      <c r="T6" s="190"/>
+      <c r="U6" s="191"/>
+      <c r="V6" s="192"/>
+      <c r="W6" s="193"/>
+      <c r="X6" s="194"/>
+      <c r="Y6" s="195"/>
+      <c r="Z6" s="196"/>
+      <c r="AA6" s="197"/>
+      <c r="AB6" s="198"/>
+      <c r="AC6" s="199"/>
+      <c r="AD6" s="200"/>
+      <c r="AE6" s="201"/>
+      <c r="AF6" s="202"/>
+      <c r="AG6" s="203"/>
       <c r="AH6" s="204"/>
     </row>
     <row r="7">
-      <c r="A7" s="205" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="206" t="inlineStr">
-        <is>
-          <t>Зуев Сергей Константинович</t>
-        </is>
-      </c>
-      <c r="C7" s="2078"/>
-      <c r="D7" s="2082"/>
-      <c r="E7" s="2086"/>
-      <c r="F7" s="2090"/>
-      <c r="G7" s="2094"/>
-      <c r="H7" s="2098"/>
-      <c r="I7" s="2102"/>
-      <c r="J7" s="2106"/>
-      <c r="K7" s="2110"/>
-      <c r="L7" s="2114"/>
-      <c r="M7" s="2118"/>
-      <c r="N7" s="2122"/>
-      <c r="O7" s="2126"/>
-      <c r="P7" s="2130"/>
-      <c r="Q7" s="2134"/>
-      <c r="R7" s="2138"/>
-      <c r="S7" s="2142"/>
-      <c r="T7" s="2146"/>
-      <c r="U7" s="2150"/>
-      <c r="V7" s="2154"/>
-      <c r="W7" s="2158"/>
-      <c r="X7" s="2162"/>
-      <c r="Y7" s="2166"/>
-      <c r="Z7" s="2170"/>
-      <c r="AA7" s="2174"/>
-      <c r="AB7" s="2178"/>
-      <c r="AC7" s="2182"/>
-      <c r="AD7" s="2186"/>
-      <c r="AE7" s="2190"/>
-      <c r="AF7" s="2194"/>
-      <c r="AG7" s="2198"/>
+      <c r="A7" s="205"/>
+      <c r="B7" s="206"/>
+      <c r="C7" s="207"/>
+      <c r="D7" s="208"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="210"/>
+      <c r="G7" s="211"/>
+      <c r="H7" s="212"/>
+      <c r="I7" s="213"/>
+      <c r="J7" s="214"/>
+      <c r="K7" s="215"/>
+      <c r="L7" s="216"/>
+      <c r="M7" s="217"/>
+      <c r="N7" s="218"/>
+      <c r="O7" s="219"/>
+      <c r="P7" s="220"/>
+      <c r="Q7" s="221"/>
+      <c r="R7" s="222"/>
+      <c r="S7" s="223"/>
+      <c r="T7" s="224"/>
+      <c r="U7" s="225"/>
+      <c r="V7" s="226"/>
+      <c r="W7" s="227"/>
+      <c r="X7" s="228"/>
+      <c r="Y7" s="229"/>
+      <c r="Z7" s="230"/>
+      <c r="AA7" s="231"/>
+      <c r="AB7" s="232"/>
+      <c r="AC7" s="233"/>
+      <c r="AD7" s="234"/>
+      <c r="AE7" s="235"/>
+      <c r="AF7" s="236"/>
+      <c r="AG7" s="237"/>
       <c r="AH7" s="238"/>
     </row>
     <row r="8">
-      <c r="A8" s="239" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B8" s="240" t="inlineStr">
-        <is>
-          <t>Абенд Евгений Сергеевич</t>
-        </is>
-      </c>
-      <c r="C8" s="2202"/>
-      <c r="D8" s="2206"/>
-      <c r="E8" s="2210"/>
-      <c r="F8" s="2214"/>
-      <c r="G8" s="2218"/>
-      <c r="H8" s="2222"/>
-      <c r="I8" s="2226"/>
-      <c r="J8" s="2230"/>
-      <c r="K8" s="2234"/>
-      <c r="L8" s="2238"/>
-      <c r="M8" s="2242"/>
-      <c r="N8" s="2246"/>
-      <c r="O8" s="2250"/>
-      <c r="P8" s="2254"/>
-      <c r="Q8" s="2258"/>
-      <c r="R8" s="2262"/>
-      <c r="S8" s="2266"/>
-      <c r="T8" s="2270"/>
-      <c r="U8" s="2274"/>
-      <c r="V8" s="2278"/>
-      <c r="W8" s="2282"/>
-      <c r="X8" s="2286"/>
-      <c r="Y8" s="2290"/>
-      <c r="Z8" s="2294"/>
-      <c r="AA8" s="2298"/>
-      <c r="AB8" s="2302"/>
-      <c r="AC8" s="2306"/>
-      <c r="AD8" s="2310"/>
-      <c r="AE8" s="2314"/>
-      <c r="AF8" s="2318"/>
-      <c r="AG8" s="2322"/>
+      <c r="A8" s="239"/>
+      <c r="B8" s="240"/>
+      <c r="C8" s="241"/>
+      <c r="D8" s="242"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="244"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="246"/>
+      <c r="I8" s="247"/>
+      <c r="J8" s="248"/>
+      <c r="K8" s="249"/>
+      <c r="L8" s="250"/>
+      <c r="M8" s="251"/>
+      <c r="N8" s="252"/>
+      <c r="O8" s="253"/>
+      <c r="P8" s="254"/>
+      <c r="Q8" s="255"/>
+      <c r="R8" s="256"/>
+      <c r="S8" s="257"/>
+      <c r="T8" s="258"/>
+      <c r="U8" s="259"/>
+      <c r="V8" s="260"/>
+      <c r="W8" s="261"/>
+      <c r="X8" s="262"/>
+      <c r="Y8" s="263"/>
+      <c r="Z8" s="264"/>
+      <c r="AA8" s="265"/>
+      <c r="AB8" s="266"/>
+      <c r="AC8" s="267"/>
+      <c r="AD8" s="268"/>
+      <c r="AE8" s="269"/>
+      <c r="AF8" s="270"/>
+      <c r="AG8" s="271"/>
       <c r="AH8" s="272"/>
     </row>
     <row r="9">
-      <c r="A9" s="273" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="274" t="inlineStr">
-        <is>
-          <t>Болгаров Вениамин Владимирович</t>
-        </is>
-      </c>
-      <c r="C9" s="2326"/>
-      <c r="D9" s="2330"/>
-      <c r="E9" s="2334"/>
-      <c r="F9" s="2338"/>
-      <c r="G9" s="2342"/>
-      <c r="H9" s="2346"/>
-      <c r="I9" s="2350"/>
-      <c r="J9" s="2354"/>
-      <c r="K9" s="2358"/>
-      <c r="L9" s="2362"/>
-      <c r="M9" s="2366"/>
-      <c r="N9" s="2370"/>
-      <c r="O9" s="2374"/>
-      <c r="P9" s="2378"/>
-      <c r="Q9" s="2382"/>
-      <c r="R9" s="2386"/>
-      <c r="S9" s="2390"/>
-      <c r="T9" s="2394"/>
-      <c r="U9" s="2398"/>
-      <c r="V9" s="2402"/>
-      <c r="W9" s="2406"/>
-      <c r="X9" s="2410"/>
-      <c r="Y9" s="2414"/>
-      <c r="Z9" s="2418"/>
-      <c r="AA9" s="2422"/>
-      <c r="AB9" s="2426"/>
-      <c r="AC9" s="2430"/>
-      <c r="AD9" s="2434"/>
-      <c r="AE9" s="2438"/>
-      <c r="AF9" s="2442"/>
-      <c r="AG9" s="2446"/>
+      <c r="A9" s="273"/>
+      <c r="B9" s="274"/>
+      <c r="C9" s="275"/>
+      <c r="D9" s="276"/>
+      <c r="E9" s="277"/>
+      <c r="F9" s="278"/>
+      <c r="G9" s="279"/>
+      <c r="H9" s="280"/>
+      <c r="I9" s="281"/>
+      <c r="J9" s="282"/>
+      <c r="K9" s="283"/>
+      <c r="L9" s="284"/>
+      <c r="M9" s="285"/>
+      <c r="N9" s="286"/>
+      <c r="O9" s="287"/>
+      <c r="P9" s="288"/>
+      <c r="Q9" s="289"/>
+      <c r="R9" s="290"/>
+      <c r="S9" s="291"/>
+      <c r="T9" s="292"/>
+      <c r="U9" s="293"/>
+      <c r="V9" s="294"/>
+      <c r="W9" s="295"/>
+      <c r="X9" s="296"/>
+      <c r="Y9" s="297"/>
+      <c r="Z9" s="298"/>
+      <c r="AA9" s="299"/>
+      <c r="AB9" s="300"/>
+      <c r="AC9" s="301"/>
+      <c r="AD9" s="302"/>
+      <c r="AE9" s="303"/>
+      <c r="AF9" s="304"/>
+      <c r="AG9" s="305"/>
       <c r="AH9" s="306"/>
     </row>
     <row r="10">
-      <c r="A10" s="307" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B10" s="308" t="inlineStr">
-        <is>
-          <t>Губайдулин Вадим Ринатович</t>
-        </is>
-      </c>
-      <c r="C10" s="2450"/>
-      <c r="D10" s="2454"/>
-      <c r="E10" s="2458"/>
-      <c r="F10" s="2462"/>
-      <c r="G10" s="2466"/>
-      <c r="H10" s="2470"/>
-      <c r="I10" s="2474"/>
-      <c r="J10" s="2478"/>
-      <c r="K10" s="2482"/>
-      <c r="L10" s="2486"/>
-      <c r="M10" s="2490"/>
-      <c r="N10" s="2494"/>
-      <c r="O10" s="2498"/>
-      <c r="P10" s="2502"/>
-      <c r="Q10" s="2506"/>
-      <c r="R10" s="2510"/>
-      <c r="S10" s="2514"/>
-      <c r="T10" s="2518"/>
-      <c r="U10" s="2522"/>
-      <c r="V10" s="2526"/>
-      <c r="W10" s="2530"/>
-      <c r="X10" s="2534"/>
-      <c r="Y10" s="2538"/>
-      <c r="Z10" s="2542"/>
-      <c r="AA10" s="2546"/>
-      <c r="AB10" s="2550"/>
-      <c r="AC10" s="2554"/>
-      <c r="AD10" s="2558"/>
-      <c r="AE10" s="2562"/>
-      <c r="AF10" s="2566"/>
-      <c r="AG10" s="2570"/>
+      <c r="A10" s="307"/>
+      <c r="B10" s="308"/>
+      <c r="C10" s="309"/>
+      <c r="D10" s="310"/>
+      <c r="E10" s="311"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="313"/>
+      <c r="H10" s="314"/>
+      <c r="I10" s="315"/>
+      <c r="J10" s="316"/>
+      <c r="K10" s="317"/>
+      <c r="L10" s="318"/>
+      <c r="M10" s="319"/>
+      <c r="N10" s="320"/>
+      <c r="O10" s="321"/>
+      <c r="P10" s="322"/>
+      <c r="Q10" s="323"/>
+      <c r="R10" s="324"/>
+      <c r="S10" s="325"/>
+      <c r="T10" s="326"/>
+      <c r="U10" s="327"/>
+      <c r="V10" s="328"/>
+      <c r="W10" s="329"/>
+      <c r="X10" s="330"/>
+      <c r="Y10" s="331"/>
+      <c r="Z10" s="332"/>
+      <c r="AA10" s="333"/>
+      <c r="AB10" s="334"/>
+      <c r="AC10" s="335"/>
+      <c r="AD10" s="336"/>
+      <c r="AE10" s="337"/>
+      <c r="AF10" s="338"/>
+      <c r="AG10" s="339"/>
       <c r="AH10" s="340"/>
     </row>
     <row r="11">
-      <c r="A11" s="341" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B11" s="342" t="inlineStr">
-        <is>
-          <t>Даниленко Никита Геннадьевич</t>
-        </is>
-      </c>
-      <c r="C11" s="2574"/>
-      <c r="D11" s="2578"/>
-      <c r="E11" s="2582"/>
-      <c r="F11" s="2586"/>
-      <c r="G11" s="2590"/>
-      <c r="H11" s="2594"/>
-      <c r="I11" s="2598"/>
-      <c r="J11" s="2602"/>
-      <c r="K11" s="2606"/>
-      <c r="L11" s="2610"/>
-      <c r="M11" s="2614"/>
-      <c r="N11" s="2618"/>
-      <c r="O11" s="2622"/>
-      <c r="P11" s="2626"/>
-      <c r="Q11" s="2630"/>
-      <c r="R11" s="2634"/>
-      <c r="S11" s="2638"/>
-      <c r="T11" s="2642"/>
-      <c r="U11" s="2646"/>
-      <c r="V11" s="2650"/>
-      <c r="W11" s="2654"/>
-      <c r="X11" s="2658"/>
-      <c r="Y11" s="2662"/>
-      <c r="Z11" s="2666"/>
-      <c r="AA11" s="2670"/>
-      <c r="AB11" s="2674"/>
-      <c r="AC11" s="2678"/>
-      <c r="AD11" s="2682"/>
-      <c r="AE11" s="2686"/>
-      <c r="AF11" s="2690"/>
-      <c r="AG11" s="2694"/>
+      <c r="A11" s="341"/>
+      <c r="B11" s="342"/>
+      <c r="C11" s="343"/>
+      <c r="D11" s="344"/>
+      <c r="E11" s="345"/>
+      <c r="F11" s="346"/>
+      <c r="G11" s="347"/>
+      <c r="H11" s="348"/>
+      <c r="I11" s="349"/>
+      <c r="J11" s="350"/>
+      <c r="K11" s="351"/>
+      <c r="L11" s="352"/>
+      <c r="M11" s="353"/>
+      <c r="N11" s="354"/>
+      <c r="O11" s="355"/>
+      <c r="P11" s="356"/>
+      <c r="Q11" s="357"/>
+      <c r="R11" s="358"/>
+      <c r="S11" s="359"/>
+      <c r="T11" s="360"/>
+      <c r="U11" s="361"/>
+      <c r="V11" s="362"/>
+      <c r="W11" s="363"/>
+      <c r="X11" s="364"/>
+      <c r="Y11" s="365"/>
+      <c r="Z11" s="366"/>
+      <c r="AA11" s="367"/>
+      <c r="AB11" s="368"/>
+      <c r="AC11" s="369"/>
+      <c r="AD11" s="370"/>
+      <c r="AE11" s="371"/>
+      <c r="AF11" s="372"/>
+      <c r="AG11" s="373"/>
       <c r="AH11" s="374"/>
     </row>
     <row r="12">
-      <c r="A12" s="375" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B12" s="376" t="inlineStr">
-        <is>
-          <t>Долгов Сергей Александрович</t>
-        </is>
-      </c>
-      <c r="C12" s="2698"/>
-      <c r="D12" s="2702"/>
-      <c r="E12" s="2706"/>
-      <c r="F12" s="2710"/>
-      <c r="G12" s="2714"/>
-      <c r="H12" s="2718"/>
-      <c r="I12" s="2722"/>
-      <c r="J12" s="2726"/>
-      <c r="K12" s="2730"/>
-      <c r="L12" s="2734"/>
-      <c r="M12" s="2738"/>
-      <c r="N12" s="2742"/>
-      <c r="O12" s="2746"/>
-      <c r="P12" s="2750"/>
-      <c r="Q12" s="2754"/>
-      <c r="R12" s="2758"/>
-      <c r="S12" s="2762"/>
-      <c r="T12" s="2766"/>
-      <c r="U12" s="2770"/>
-      <c r="V12" s="2774"/>
-      <c r="W12" s="2778"/>
-      <c r="X12" s="2782"/>
-      <c r="Y12" s="2786"/>
-      <c r="Z12" s="2790"/>
-      <c r="AA12" s="2794"/>
-      <c r="AB12" s="2798"/>
-      <c r="AC12" s="2802"/>
-      <c r="AD12" s="2806"/>
-      <c r="AE12" s="2810"/>
-      <c r="AF12" s="2814"/>
-      <c r="AG12" s="2818"/>
+      <c r="A12" s="375"/>
+      <c r="B12" s="376"/>
+      <c r="C12" s="377"/>
+      <c r="D12" s="378"/>
+      <c r="E12" s="379"/>
+      <c r="F12" s="380"/>
+      <c r="G12" s="381"/>
+      <c r="H12" s="382"/>
+      <c r="I12" s="383"/>
+      <c r="J12" s="384"/>
+      <c r="K12" s="385"/>
+      <c r="L12" s="386"/>
+      <c r="M12" s="387"/>
+      <c r="N12" s="388"/>
+      <c r="O12" s="389"/>
+      <c r="P12" s="390"/>
+      <c r="Q12" s="391"/>
+      <c r="R12" s="392"/>
+      <c r="S12" s="393"/>
+      <c r="T12" s="394"/>
+      <c r="U12" s="395"/>
+      <c r="V12" s="396"/>
+      <c r="W12" s="397"/>
+      <c r="X12" s="398"/>
+      <c r="Y12" s="399"/>
+      <c r="Z12" s="400"/>
+      <c r="AA12" s="401"/>
+      <c r="AB12" s="402"/>
+      <c r="AC12" s="403"/>
+      <c r="AD12" s="404"/>
+      <c r="AE12" s="405"/>
+      <c r="AF12" s="406"/>
+      <c r="AG12" s="407"/>
       <c r="AH12" s="408"/>
     </row>
     <row r="13">

</xml_diff>